<commit_message>
Fixes invalid payment reduction for account receivables.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_retur_jual.xlsx
+++ b/test/integration/project/data_retur_jual.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="27" activeTab="35"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="202">
   <si>
     <t>id</t>
   </si>
@@ -637,6 +637,27 @@
   </si>
   <si>
     <t>KlaimServis</t>
+  </si>
+  <si>
+    <t>Mr. Unknown</t>
+  </si>
+  <si>
+    <t>000005/042014/SA</t>
+  </si>
+  <si>
+    <t>000006/042014/SA</t>
+  </si>
+  <si>
+    <t>000006-SJ-KB-052014</t>
+  </si>
+  <si>
+    <t>000007-SJ-KB-062014</t>
+  </si>
+  <si>
+    <t>Unknown Destination</t>
+  </si>
+  <si>
+    <t>AB-222</t>
   </si>
 </sst>
 </file>
@@ -1341,10 +1362,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1531,6 +1552,70 @@
         <v>-3</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="1">
+        <v>41965</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="1">
+        <v>41965</v>
+      </c>
+      <c r="H7" s="1">
+        <v>41965</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>118</v>
+      </c>
+      <c r="L7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="1">
+        <v>41965</v>
+      </c>
+      <c r="E8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="1">
+        <v>41965</v>
+      </c>
+      <c r="H8" s="1">
+        <v>41965</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>118</v>
+      </c>
+      <c r="L8">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1540,10 +1625,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1638,6 +1723,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-6</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-7</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1647,10 +1760,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1825,6 +1938,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41692</v>
+      </c>
+      <c r="C6">
+        <v>99999</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6">
+        <v>-1</v>
+      </c>
+      <c r="J6">
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1834,10 +1976,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1884,6 +2026,22 @@
       </c>
       <c r="B5">
         <v>-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-5</v>
+      </c>
+      <c r="B7">
+        <v>-9</v>
       </c>
     </row>
   </sheetData>
@@ -1935,10 +2093,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1993,6 +2151,17 @@
         <v>-3</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-5</v>
+      </c>
+      <c r="B5">
+        <v>10000</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2002,10 +2171,10 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2072,6 +2241,29 @@
         <v>127</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41967</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="1">
+        <v>41973</v>
+      </c>
+      <c r="H3">
+        <v>100000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2081,18 +2273,17 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2153,6 +2344,34 @@
       </c>
       <c r="D4">
         <v>20000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41967</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41967</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
@@ -2260,10 +2479,10 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20"/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2322,6 +2541,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-4</v>
+      </c>
+      <c r="B3">
+        <v>-2</v>
+      </c>
+      <c r="C3">
+        <v>70000</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>41967</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2331,10 +2570,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2659,6 +2898,82 @@
         <v>-3</v>
       </c>
       <c r="R8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9">
+        <v>-8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="1">
+        <v>41967</v>
+      </c>
+      <c r="H9" s="1">
+        <v>41967</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="M9" s="1">
+        <v>41973</v>
+      </c>
+      <c r="N9">
+        <v>-6</v>
+      </c>
+      <c r="P9">
+        <v>-5</v>
+      </c>
+      <c r="Q9">
+        <v>-4</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10">
+        <v>-9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>197</v>
+      </c>
+      <c r="G10" s="1">
+        <v>41967</v>
+      </c>
+      <c r="H10" s="1">
+        <v>41967</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="M10" s="1">
+        <v>41973</v>
+      </c>
+      <c r="N10">
+        <v>-7</v>
+      </c>
+      <c r="P10">
+        <v>-5</v>
+      </c>
+      <c r="Q10">
+        <v>-5</v>
+      </c>
+      <c r="R10" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2798,10 +3113,10 @@
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet24"/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:H8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3009,6 +3324,40 @@
         <v>-1</v>
       </c>
       <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>-8</v>
+      </c>
+      <c r="D12">
+        <v>10000</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>-1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>-9</v>
+      </c>
+      <c r="D13">
+        <v>10000</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>-1</v>
+      </c>
+      <c r="H13">
         <v>0</v>
       </c>
     </row>
@@ -4322,8 +4671,8 @@
   <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add `bisaDijualKembali` to `ReturJual`.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_retur_jual.xlsx
+++ b/test/integration/project/data_retur_jual.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="34" activeTab="39"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" firstSheet="26" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="215">
   <si>
     <t>id</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>kategoriKas_id</t>
+  </si>
+  <si>
+    <t>bisaDijualKembali</t>
   </si>
 </sst>
 </file>
@@ -3523,10 +3526,10 @@
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet27"/>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3542,9 +3545,10 @@
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -3590,8 +3594,11 @@
       <c r="O1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -3622,8 +3629,11 @@
       <c r="M2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -3653,6 +3663,9 @@
       </c>
       <c r="M3">
         <v>-1</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5167,7 +5180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>